<commit_message>
write to excel callback added
</commit_message>
<xml_diff>
--- a/myExcel.xlsx
+++ b/myExcel.xlsx
@@ -12,9 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Madhav</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
   <si>
     <t>1</t>
@@ -42,27 +48,6 @@
   </si>
   <si>
     <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
   </si>
 </sst>
 </file>
@@ -107,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,32 +102,32 @@
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s" s="0">
         <v>8</v>
       </c>
     </row>
@@ -156,22 +141,104 @@
       <c r="C4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>16</v>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>